<commit_message>
Code Notebook v1 uploaded
</commit_message>
<xml_diff>
--- a/Datasets/Recruitment_Predictive_Model_Dataset/Recruitment_Predictive_Model_Dataset.xlsx
+++ b/Datasets/Recruitment_Predictive_Model_Dataset/Recruitment_Predictive_Model_Dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Drive\Academics\Visiting Lectures\2026-H1\2026H1-IITP-EMBA-MB548\2026-H2-IITP-EMBA-MB548\Datasets\Recruitment_Predictive_Model_Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A97781B-8B32-4050-96E6-CC501E27D62C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D51C1720-2AF3-43FC-A72F-EA595A64AFC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recruitment_Data" sheetId="1" r:id="rId1"/>
@@ -3566,7 +3566,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -41631,8 +41633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>